<commit_message>
results updated after the changes
</commit_message>
<xml_diff>
--- a/results/2099 - wyniki/2099 - podsumowanie.xlsx
+++ b/results/2099 - wyniki/2099 - podsumowanie.xlsx
@@ -12,6 +12,9 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hobby i przyjemności" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transport i noclegi" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Podróże" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Abonamenty i usługi" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Leki i zdrowie" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Książki i nauka" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -48,7 +51,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -63,17 +66,41 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -379,7 +406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -390,6 +417,9 @@
     <col customWidth="1" max="2" min="2" width="14"/>
     <col customWidth="1" max="3" min="3" width="14"/>
     <col customWidth="1" max="4" min="4" width="14"/>
+    <col customWidth="1" max="5" min="5" width="14"/>
+    <col customWidth="1" max="8" min="8" width="10"/>
+    <col customWidth="1" max="9" min="9" width="18"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -409,6 +439,17 @@
           <t>Przychody [zł]:</t>
         </is>
       </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Nadwyżki [zł]:</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Całkowita nadwyżka przychodów:</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -425,6 +466,19 @@
       <c r="D2" s="1" t="n">
         <v>3950</v>
       </c>
+      <c r="E2" s="1" t="n">
+        <v>1210.81</v>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>[zł]</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>[% przychodów]</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -441,6 +495,15 @@
       <c r="D3" s="1" t="n">
         <v>4122.5</v>
       </c>
+      <c r="E3" s="1" t="n">
+        <v>1109.1</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>14529.77</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>30.65</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -457,8 +520,17 @@
       <c r="D4" s="1" t="n">
         <v>593.63</v>
       </c>
+      <c r="E4" s="1" t="n">
+        <v>884.89</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
@@ -485,7 +557,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Styczeń  - 350zł</t>
         </is>
@@ -507,12 +579,12 @@
       <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -577,7 +649,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Luty  - 330zł</t>
         </is>
@@ -585,12 +657,12 @@
       <c r="B4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -617,7 +689,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>Marzec  - 200zł</t>
         </is>
@@ -625,12 +697,12 @@
       <c r="B8" s="1" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B9" s="5" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -647,7 +719,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>Kwiecień  - 290zł</t>
         </is>
@@ -655,12 +727,12 @@
       <c r="B11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="inlineStr">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -697,7 +769,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>Czerwiec  - 2500zł</t>
         </is>
@@ -705,12 +777,12 @@
       <c r="B16" s="1" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B17" s="5" t="inlineStr">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -727,7 +799,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>Lipiec  - 220zł</t>
         </is>
@@ -735,12 +807,12 @@
       <c r="B19" s="1" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B20" s="5" t="inlineStr">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -767,7 +839,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
+      <c r="A23" s="5" t="inlineStr">
         <is>
           <t>Sierpień  - 430zł</t>
         </is>
@@ -775,12 +847,12 @@
       <c r="B23" s="1" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B24" s="5" t="inlineStr">
+      <c r="A24" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B24" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -807,7 +879,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="inlineStr">
+      <c r="A27" s="5" t="inlineStr">
         <is>
           <t>Wrzesień  - 850zł</t>
         </is>
@@ -815,12 +887,12 @@
       <c r="B27" s="1" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B28" s="5" t="inlineStr">
+      <c r="A28" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B28" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -857,7 +929,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="inlineStr">
+      <c r="A32" s="5" t="inlineStr">
         <is>
           <t>Październik  - 99zł</t>
         </is>
@@ -865,12 +937,12 @@
       <c r="B32" s="1" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B33" s="5" t="inlineStr">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -887,7 +959,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="inlineStr">
+      <c r="A35" s="5" t="inlineStr">
         <is>
           <t>Listopad  - 70zł</t>
         </is>
@@ -895,12 +967,12 @@
       <c r="B35" s="1" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B36" s="5" t="inlineStr">
+      <c r="A36" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B36" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -917,7 +989,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="inlineStr">
+      <c r="A38" s="5" t="inlineStr">
         <is>
           <t>Grudzień  - 80zł</t>
         </is>
@@ -925,12 +997,12 @@
       <c r="B38" s="1" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B39" s="5" t="inlineStr">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B39" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -988,7 +1060,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Styczeń  - 124zł</t>
         </is>
@@ -1010,12 +1082,12 @@
       <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1100,7 +1172,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Luty  - 117zł</t>
         </is>
@@ -1108,12 +1180,12 @@
       <c r="B6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1150,7 +1222,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
+      <c r="A11" s="5" t="inlineStr">
         <is>
           <t>Marzec  - 105zł</t>
         </is>
@@ -1158,12 +1230,12 @@
       <c r="B11" s="1" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B12" s="5" t="inlineStr">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B12" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1190,7 +1262,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="inlineStr">
+      <c r="A15" s="5" t="inlineStr">
         <is>
           <t>Kwiecień  - 80zł</t>
         </is>
@@ -1198,12 +1270,12 @@
       <c r="B15" s="1" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B16" s="5" t="inlineStr">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1220,7 +1292,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" s="5" t="inlineStr">
         <is>
           <t>Maj  - 104zł</t>
         </is>
@@ -1228,12 +1300,12 @@
       <c r="B18" s="1" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B19" s="5" t="inlineStr">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1260,7 +1332,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>Czerwiec  - 180zł</t>
         </is>
@@ -1268,12 +1340,12 @@
       <c r="B22" s="1" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B23" s="5" t="inlineStr">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1300,7 +1372,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="inlineStr">
+      <c r="A26" s="5" t="inlineStr">
         <is>
           <t>Lipiec  - 20zł</t>
         </is>
@@ -1308,12 +1380,12 @@
       <c r="B26" s="1" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B27" s="5" t="inlineStr">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1330,7 +1402,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="inlineStr">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>Sierpień  - 42zł</t>
         </is>
@@ -1338,12 +1410,12 @@
       <c r="B29" s="1" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B30" s="5" t="inlineStr">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1370,7 +1442,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="inlineStr">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t>Październik  - 90zł</t>
         </is>
@@ -1378,12 +1450,12 @@
       <c r="B33" s="1" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B34" s="5" t="inlineStr">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1400,7 +1472,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="inlineStr">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>Grudzień  - 70zł</t>
         </is>
@@ -1408,12 +1480,12 @@
       <c r="B36" s="1" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B37" s="5" t="inlineStr">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1480,7 +1552,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Styczeń  - 117zł</t>
         </is>
@@ -1502,12 +1574,12 @@
       <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1592,7 +1664,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Luty  - 192zł</t>
         </is>
@@ -1600,12 +1672,12 @@
       <c r="B6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1652,7 +1724,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
+      <c r="A12" s="5" t="inlineStr">
         <is>
           <t>Marzec  - 65zł</t>
         </is>
@@ -1660,12 +1732,12 @@
       <c r="B12" s="1" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B13" s="5" t="inlineStr">
+      <c r="A13" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B13" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1692,7 +1764,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
         <is>
           <t>Kwiecień  - 50zł</t>
         </is>
@@ -1700,12 +1772,12 @@
       <c r="B16" s="1" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B17" s="5" t="inlineStr">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1722,7 +1794,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
+      <c r="A19" s="5" t="inlineStr">
         <is>
           <t>Maj  - 50zł</t>
         </is>
@@ -1730,12 +1802,12 @@
       <c r="B19" s="1" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B20" s="5" t="inlineStr">
+      <c r="A20" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B20" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1752,7 +1824,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
         <is>
           <t>Czerwiec  - 90zł</t>
         </is>
@@ -1760,12 +1832,12 @@
       <c r="B22" s="1" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B23" s="5" t="inlineStr">
+      <c r="A23" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B23" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1792,7 +1864,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="inlineStr">
+      <c r="A26" s="5" t="inlineStr">
         <is>
           <t>Lipiec  - 40zł</t>
         </is>
@@ -1800,12 +1872,12 @@
       <c r="B26" s="1" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B27" s="5" t="inlineStr">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1822,7 +1894,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="inlineStr">
+      <c r="A29" s="5" t="inlineStr">
         <is>
           <t>Wrzesień  - 85zł</t>
         </is>
@@ -1830,12 +1902,12 @@
       <c r="B29" s="1" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B30" s="5" t="inlineStr">
+      <c r="A30" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B30" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1862,7 +1934,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="inlineStr">
+      <c r="A33" s="5" t="inlineStr">
         <is>
           <t>Październik  - 40zł</t>
         </is>
@@ -1870,12 +1942,12 @@
       <c r="B33" s="1" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B34" s="5" t="inlineStr">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1892,7 +1964,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="inlineStr">
+      <c r="A36" s="5" t="inlineStr">
         <is>
           <t>Listopad  - 85zł</t>
         </is>
@@ -1900,12 +1972,12 @@
       <c r="B36" s="1" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B37" s="5" t="inlineStr">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -1932,7 +2004,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="inlineStr">
+      <c r="A40" s="5" t="inlineStr">
         <is>
           <t>Grudzień  - 75zł</t>
         </is>
@@ -1940,12 +2012,12 @@
       <c r="B40" s="1" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B41" s="5" t="inlineStr">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -2013,7 +2085,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Maj  - 470zł</t>
         </is>
@@ -2035,12 +2107,12 @@
       <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -2125,7 +2197,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>Sierpień  - 770zł</t>
         </is>
@@ -2133,12 +2205,12 @@
       <c r="B6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -2195,7 +2267,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
         <is>
           <t>Październik  - 1250zł</t>
         </is>
@@ -2203,12 +2275,12 @@
       <c r="B13" s="1" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B14" s="5" t="inlineStr">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -2245,7 +2317,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
+      <c r="A18" s="5" t="inlineStr">
         <is>
           <t>Grudzień  - 200zł</t>
         </is>
@@ -2253,12 +2325,12 @@
       <c r="B18" s="1" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="5" t="inlineStr">
-        <is>
-          <t>Co?</t>
-        </is>
-      </c>
-      <c r="B19" s="5" t="inlineStr">
+      <c r="A19" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B19" s="6" t="inlineStr">
         <is>
           <t>Kwota [zł]</t>
         </is>
@@ -2295,4 +2367,1163 @@
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="9"/>
+    <col customWidth="1" max="7" min="7" width="14"/>
+    <col customWidth="1" max="8" min="8" width="14"/>
+    <col customWidth="1" max="12" min="12" width="14"/>
+    <col customWidth="1" max="13" min="13" width="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Styczeń  - 45zł</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Dla sum miesięcznych:</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>56.67</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>65</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>20.75</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>23.45</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>5.1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Luty  - 65zł</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>hbo go</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Marzec  - 65zł</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>hbo go</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>Kwiecień  - 65zł</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B16" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>hbo go</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>Maj  - 105zł</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B21" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>hbo go</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>fryzjer</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5" t="inlineStr">
+        <is>
+          <t>Czerwiec  - 45zł</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="n"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B27" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="5" t="inlineStr">
+        <is>
+          <t>Lipiec  - 25zł</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="5" t="inlineStr">
+        <is>
+          <t>Sierpień  - 25zł</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="n"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B34" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="5" t="inlineStr">
+        <is>
+          <t>Wrzesień  - 65zł</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="n"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>fryzjer</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="5" t="inlineStr">
+        <is>
+          <t>Październik  - 45zł</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="n"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="5" t="inlineStr">
+        <is>
+          <t>Listopad  - 65zł</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="n"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>hbo go</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="5" t="inlineStr">
+        <is>
+          <t>Grudzień  - 65zł</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="n"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B50" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>telefon</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>spotify</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>hbo go</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="7" min="7" width="14"/>
+    <col customWidth="1" max="8" min="8" width="14"/>
+    <col customWidth="1" max="12" min="12" width="14"/>
+    <col customWidth="1" max="13" min="13" width="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Styczeń  - 24zł</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Dla sum miesięcznych:</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>apteka</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>20.08</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>32.46</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>40.17</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>36.06</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Kwiecień  - 18zł</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>apteka</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Maj  - 34zł</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>apteka</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Lipiec  - 120zł</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>dentysta</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Listopad  - 20zł</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>apteka</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>Grudzień  - 25zł</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="n"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B17" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>apteka</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="24"/>
+    <col customWidth="1" max="7" min="7" width="14"/>
+    <col customWidth="1" max="8" min="8" width="14"/>
+    <col customWidth="1" max="12" min="12" width="14"/>
+    <col customWidth="1" max="13" min="13" width="14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Luty  - 90zł</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n"/>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Dla sum miesięcznych:</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="n"/>
+      <c r="N1" s="2" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="N2" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>kurs internetowy 'xyz'</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>30.42</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="n">
+        <v>41.46</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>31.87</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>Kwiecień  - 40zł</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>książka 'xyz'</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Maj  - 80zł</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>książka 'wxy'</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>Sierpień  - 120zł</t>
+        </is>
+      </c>
+      <c r="B10" s="1" t="n"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B11" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>kurs internetowy 'wxy'</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Listopad  - 35zł</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="inlineStr">
+        <is>
+          <t>Co?</t>
+        </is>
+      </c>
+      <c r="B14" s="6" t="inlineStr">
+        <is>
+          <t>Kwota [zł]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>książka 'wxyz'</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
results adjusted after changes in the code
</commit_message>
<xml_diff>
--- a/results/2099 - wyniki/2099 - podsumowanie.xlsx
+++ b/results/2099 - wyniki/2099 - podsumowanie.xlsx
@@ -541,7 +541,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,8 +552,6 @@
     <col customWidth="1" max="1" min="1" width="23"/>
     <col customWidth="1" max="7" min="7" width="14"/>
     <col customWidth="1" max="8" min="8" width="14"/>
-    <col customWidth="1" max="12" min="12" width="14"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -570,13 +568,6 @@
       </c>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Dla wydatków indywidualnych:</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -604,21 +595,6 @@
           <t>Std [zł]:</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Średnia [zł]:</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>Mediana [zł]:</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>Std [zł]:</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -638,15 +614,6 @@
       <c r="I3" s="2" t="n">
         <v>654.17</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>301.06</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>135</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>549.1900000000001</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
@@ -687,6 +654,13 @@
       <c r="B7" s="1" t="n">
         <v>50</v>
       </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="5" t="inlineStr">
@@ -695,6 +669,21 @@
         </is>
       </c>
       <c r="B8" s="1" t="n"/>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="6" t="inlineStr">
@@ -706,6 +695,15 @@
         <is>
           <t>Kwota [zł]</t>
         </is>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>301.06</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>549.1900000000001</v>
       </c>
     </row>
     <row r="10">
@@ -1032,7 +1030,7 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1044,7 +1042,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1055,8 +1053,6 @@
     <col customWidth="1" max="1" min="1" width="17"/>
     <col customWidth="1" max="7" min="7" width="14"/>
     <col customWidth="1" max="8" min="8" width="14"/>
-    <col customWidth="1" max="12" min="12" width="14"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1073,13 +1069,6 @@
       </c>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Dla wydatków indywidualnych:</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -1107,21 +1096,6 @@
           <t>Std [zł]:</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Średnia [zł]:</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>Mediana [zł]:</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>Std [zł]:</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1141,15 +1115,6 @@
       <c r="I3" s="2" t="n">
         <v>52.03</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>49.05</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>36.04</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1190,6 +1155,13 @@
           <t>Kwota [zł]</t>
         </is>
       </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1200,6 +1172,21 @@
       <c r="B8" s="1" t="n">
         <v>80</v>
       </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1209,6 +1196,15 @@
       </c>
       <c r="B9" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>49.05</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>36.04</v>
       </c>
     </row>
     <row r="10">
@@ -1524,7 +1520,7 @@
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1536,7 +1532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1547,8 +1543,6 @@
     <col customWidth="1" max="1" min="1" width="15"/>
     <col customWidth="1" max="7" min="7" width="14"/>
     <col customWidth="1" max="8" min="8" width="14"/>
-    <col customWidth="1" max="12" min="12" width="14"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1565,13 +1559,6 @@
       </c>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Dla wydatków indywidualnych:</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -1599,21 +1586,6 @@
           <t>Std [zł]:</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Średnia [zł]:</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>Mediana [zł]:</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>Std [zł]:</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1633,15 +1605,6 @@
       <c r="I3" s="2" t="n">
         <v>45.91</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>42.33</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>14.67</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1682,6 +1645,13 @@
           <t>Kwota [zł]</t>
         </is>
       </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1692,6 +1662,21 @@
       <c r="B8" s="1" t="n">
         <v>50</v>
       </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1701,6 +1686,15 @@
       </c>
       <c r="B9" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>42.33</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>14.67</v>
       </c>
     </row>
     <row r="10">
@@ -2057,7 +2051,7 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -2069,7 +2063,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2080,8 +2074,6 @@
     <col customWidth="1" max="1" min="1" width="19"/>
     <col customWidth="1" max="7" min="7" width="14"/>
     <col customWidth="1" max="8" min="8" width="14"/>
-    <col customWidth="1" max="12" min="12" width="14"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2098,13 +2090,6 @@
       </c>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Dla wydatków indywidualnych:</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -2132,21 +2117,6 @@
           <t>Std [zł]:</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Średnia [zł]:</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>Mediana [zł]:</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>Std [zł]:</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2166,15 +2136,6 @@
       <c r="I3" s="2" t="n">
         <v>388.73</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>206.92</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>120</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>135.44</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2215,6 +2176,13 @@
           <t>Kwota [zł]</t>
         </is>
       </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2225,6 +2193,21 @@
       <c r="B8" s="1" t="n">
         <v>150</v>
       </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2234,6 +2217,15 @@
       </c>
       <c r="B9" s="1" t="n">
         <v>100</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>206.92</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>135.44</v>
       </c>
     </row>
     <row r="10">
@@ -2363,7 +2355,7 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -2375,7 +2367,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2386,8 +2378,6 @@
     <col customWidth="1" max="1" min="1" width="9"/>
     <col customWidth="1" max="7" min="7" width="14"/>
     <col customWidth="1" max="8" min="8" width="14"/>
-    <col customWidth="1" max="12" min="12" width="14"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2404,13 +2394,6 @@
       </c>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Dla wydatków indywidualnych:</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -2438,21 +2421,6 @@
           <t>Std [zł]:</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Średnia [zł]:</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>Mediana [zł]:</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>Std [zł]:</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2472,15 +2440,6 @@
       <c r="I3" s="2" t="n">
         <v>20.75</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>23.45</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>5.1</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2521,6 +2480,13 @@
       <c r="B7" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -2531,6 +2497,21 @@
       <c r="B8" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -2540,6 +2521,15 @@
       </c>
       <c r="B9" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>23.45</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>5.1</v>
       </c>
     </row>
     <row r="10">
@@ -2997,7 +2987,7 @@
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -3009,7 +2999,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3020,8 +3010,6 @@
     <col customWidth="1" max="1" min="1" width="10"/>
     <col customWidth="1" max="7" min="7" width="14"/>
     <col customWidth="1" max="8" min="8" width="14"/>
-    <col customWidth="1" max="12" min="12" width="14"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3038,13 +3026,6 @@
       </c>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Dla wydatków indywidualnych:</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -3072,21 +3053,6 @@
           <t>Std [zł]:</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Średnia [zł]:</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>Mediana [zł]:</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>Std [zł]:</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -3106,15 +3072,6 @@
       <c r="I3" s="2" t="n">
         <v>32.46</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>40.17</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>24.5</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>36.06</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
@@ -3153,6 +3110,13 @@
         </is>
       </c>
       <c r="B7" s="1" t="n"/>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -3165,6 +3129,21 @@
           <t>Kwota [zł]</t>
         </is>
       </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -3174,6 +3153,15 @@
       </c>
       <c r="B9" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>40.17</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>36.06</v>
       </c>
     </row>
     <row r="10">
@@ -3275,7 +3263,7 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -3287,7 +3275,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3298,8 +3286,6 @@
     <col customWidth="1" max="1" min="1" width="24"/>
     <col customWidth="1" max="7" min="7" width="14"/>
     <col customWidth="1" max="8" min="8" width="14"/>
-    <col customWidth="1" max="12" min="12" width="14"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3316,13 +3302,6 @@
       </c>
       <c r="H1" s="2" t="n"/>
       <c r="I1" s="2" t="n"/>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Dla wydatków indywidualnych:</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="n"/>
-      <c r="N1" s="2" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="inlineStr">
@@ -3350,21 +3329,6 @@
           <t>Std [zł]:</t>
         </is>
       </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>Średnia [zł]:</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>Mediana [zł]:</t>
-        </is>
-      </c>
-      <c r="N2" s="2" t="inlineStr">
-        <is>
-          <t>Std [zł]:</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -3384,15 +3348,6 @@
       <c r="I3" s="2" t="n">
         <v>41.46</v>
       </c>
-      <c r="L3" s="2" t="n">
-        <v>73</v>
-      </c>
-      <c r="M3" s="2" t="n">
-        <v>80</v>
-      </c>
-      <c r="N3" s="2" t="n">
-        <v>31.87</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="inlineStr">
@@ -3431,6 +3386,13 @@
         </is>
       </c>
       <c r="B7" s="1" t="n"/>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Dla wydatków indywidualnych:</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="n"/>
+      <c r="I7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="6" t="inlineStr">
@@ -3443,6 +3405,21 @@
           <t>Kwota [zł]</t>
         </is>
       </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Średnia [zł]:</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Mediana [zł]:</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Std [zł]:</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -3452,6 +3429,15 @@
       </c>
       <c r="B9" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>31.87</v>
       </c>
     </row>
     <row r="10">
@@ -3522,7 +3508,7 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>